<commit_message>
Update 1 - Introduction to Ribbon & Tabs.xlsx
</commit_message>
<xml_diff>
--- a/InClassWorkingFiles/1 - Introduction to Ribbon & Tabs.xlsx
+++ b/InClassWorkingFiles/1 - Introduction to Ribbon & Tabs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Excel_for_Data_Science\InClassWorkingFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4423E0CA-6697-4C42-9894-264A26ABE958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753C3517-9EF7-464B-822A-D1E8C957F70A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6ADA2516-0932-4810-B250-44A626CAFCEB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Introduction to Ribbon</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>4. Summary Functions - Sumifs, Countifs etc...</t>
+  </si>
+  <si>
+    <t>Today's Agenda</t>
   </si>
 </sst>
 </file>
@@ -146,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -161,6 +164,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -476,35 +480,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4EB9669-7E1D-4B58-ADC0-F07D6C1EBD80}">
-  <dimension ref="B5:B8"/>
+  <dimension ref="B3:J8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -515,7 +536,7 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>